<commit_message>
Added globaldata to location1.csv
</commit_message>
<xml_diff>
--- a/hmvantol/oil_sands/polyline.xlsx
+++ b/hmvantol/oil_sands/polyline.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Slope</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -89,8 +92,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,7 +150,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -170,6 +175,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -194,6 +200,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8981,11 +8988,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2134493224"/>
-        <c:axId val="2134490056"/>
+        <c:axId val="1666475880"/>
+        <c:axId val="1669251896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2134493224"/>
+        <c:axId val="1666475880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8995,12 +9002,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134490056"/>
+        <c:crossAx val="1669251896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2134490056"/>
+        <c:axId val="1669251896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9011,14 +9018,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134493224"/>
+        <c:crossAx val="1666475880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -32704,8 +32710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H484"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -42399,10 +42405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B483"/>
+  <dimension ref="A1:B485"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -42772,1079 +42778,1081 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1">
-        <v>25567.466574782753</v>
-      </c>
-      <c r="B46">
-        <v>134.72585356510081</v>
+        <f>A45+30</f>
+        <v>25475.748853894802</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1">
-        <v>25597.886875262702</v>
-      </c>
-      <c r="B47">
-        <v>134.41746875448928</v>
+        <f>A46+31</f>
+        <v>25506.748853894802</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1">
-        <v>25628.307175742648</v>
+        <v>25567.466574782753</v>
       </c>
       <c r="B48">
-        <v>133.38696547430925</v>
+        <v>134.72585356510081</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1">
-        <v>25658.727476222593</v>
+        <v>25597.886875262702</v>
       </c>
       <c r="B49">
-        <v>131.07120624431354</v>
+        <v>134.41746875448928</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1">
-        <v>25689.147776702543</v>
+        <v>25628.307175742648</v>
       </c>
       <c r="B50">
-        <v>130.76090600009576</v>
+        <v>133.38696547430925</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1">
-        <v>25719.568077182488</v>
+        <v>25658.727476222593</v>
       </c>
       <c r="B51">
-        <v>131.94655940238471</v>
+        <v>131.07120624431354</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1">
-        <v>25749.988377662434</v>
+        <v>25689.147776702543</v>
       </c>
       <c r="B52">
-        <v>132.25494421299621</v>
+        <v>130.76090600009576</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1">
-        <v>25780.408678142383</v>
+        <v>25719.568077182488</v>
       </c>
       <c r="B53">
-        <v>130.70918929272614</v>
+        <v>131.94655940238471</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1">
-        <v>25810.865497590494</v>
+        <v>25749.988377662434</v>
       </c>
       <c r="B54">
-        <v>129.88746827563091</v>
+        <v>132.25494421299621</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1">
-        <v>25841.285798070439</v>
+        <v>25780.408678142383</v>
       </c>
       <c r="B55">
-        <v>130.81262270746538</v>
+        <v>130.70918929272614</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1">
-        <v>25871.706098550385</v>
+        <v>25810.865497590494</v>
       </c>
       <c r="B56">
-        <v>134.15888521764111</v>
+        <v>129.88746827563091</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1">
-        <v>25902.126399030334</v>
+        <v>25841.285798070439</v>
       </c>
       <c r="B57">
-        <v>134.67413685773118</v>
+        <v>130.81262270746538</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1">
-        <v>25932.583218478441</v>
+        <v>25871.706098550385</v>
       </c>
       <c r="B58">
-        <v>135.4977733084327</v>
+        <v>134.15888521764111</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1">
-        <v>25963.00351895839</v>
+        <v>25902.126399030334</v>
       </c>
       <c r="B59">
-        <v>135.4977733084327</v>
+        <v>134.67413685773118</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1">
-        <v>25993.423819438336</v>
+        <v>25932.583218478441</v>
       </c>
       <c r="B60">
-        <v>135.08595508308193</v>
+        <v>135.4977733084327</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1">
-        <v>26023.844119918282</v>
+        <v>25963.00351895839</v>
       </c>
       <c r="B61">
-        <v>135.1893884978212</v>
+        <v>135.4977733084327</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1">
-        <v>26054.264420398231</v>
+        <v>25993.423819438336</v>
       </c>
       <c r="B62">
-        <v>136.06474165589236</v>
+        <v>135.08595508308193</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1">
-        <v>26084.721239846338</v>
+        <v>26023.844119918282</v>
       </c>
       <c r="B63">
-        <v>134.26231863238041</v>
+        <v>135.1893884978212</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1">
-        <v>26115.141540326287</v>
+        <v>26054.264420398231</v>
       </c>
       <c r="B64">
-        <v>133.18009864483071</v>
+        <v>136.06474165589236</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1">
-        <v>26145.561840806233</v>
+        <v>26084.721239846338</v>
       </c>
       <c r="B65">
-        <v>133.38696547430925</v>
+        <v>134.26231863238041</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1">
-        <v>26175.982141286178</v>
+        <v>26115.141540326287</v>
       </c>
       <c r="B66">
-        <v>133.38696547430925</v>
+        <v>133.18009864483071</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1">
-        <v>26206.402441766128</v>
+        <v>26145.561840806233</v>
       </c>
       <c r="B67">
-        <v>133.13029737106734</v>
+        <v>133.38696547430925</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1">
-        <v>26236.822742246073</v>
+        <v>26175.982141286178</v>
       </c>
       <c r="B68">
-        <v>128.4968634774697</v>
+        <v>133.38696547430925</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1">
-        <v>26267.243042726019</v>
+        <v>26206.402441766128</v>
       </c>
       <c r="B69">
-        <v>127.82646171527078</v>
+        <v>133.13029737106734</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1">
-        <v>26297.69986217413</v>
+        <v>26236.822742246073</v>
       </c>
       <c r="B70">
-        <v>127.20969209404778</v>
+        <v>128.4968634774697</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1">
-        <v>26328.120162654079</v>
+        <v>26267.243042726019</v>
       </c>
       <c r="B71">
-        <v>127.98161183737969</v>
+        <v>127.82646171527078</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1">
-        <v>26358.540463134024</v>
+        <v>26297.69986217413</v>
       </c>
       <c r="B72">
-        <v>128.34171335536081</v>
+        <v>127.20969209404778</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1">
-        <v>26388.96076361397</v>
+        <v>26328.120162654079</v>
       </c>
       <c r="B73">
-        <v>129.01211511755974</v>
+        <v>127.98161183737969</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1">
-        <v>26419.417583062081</v>
+        <v>26358.540463134024</v>
       </c>
       <c r="B74">
-        <v>129.06191639132308</v>
+        <v>128.34171335536081</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1">
-        <v>26449.801364573865</v>
+        <v>26388.96076361397</v>
       </c>
       <c r="B75">
-        <v>129.47373461667382</v>
+        <v>129.01211511755974</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1">
-        <v>26480.258184021975</v>
+        <v>26419.417583062081</v>
       </c>
       <c r="B76">
-        <v>129.47373461667382</v>
+        <v>129.06191639132308</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1">
-        <v>26510.678484501921</v>
+        <v>26449.801364573865</v>
       </c>
       <c r="B77">
-        <v>128.8052482880812</v>
+        <v>129.47373461667382</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1">
-        <v>26571.519085461816</v>
+        <v>26480.258184021975</v>
       </c>
       <c r="B78">
-        <v>128.8052482880812</v>
+        <v>129.47373461667382</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1">
-        <v>26601.939385941761</v>
+        <v>26510.678484501921</v>
       </c>
       <c r="B79">
-        <v>129.1136330986927</v>
+        <v>128.8052482880812</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1">
-        <v>26632.396205389872</v>
+        <v>26571.519085461816</v>
       </c>
       <c r="B80">
-        <v>129.93726954939424</v>
+        <v>128.8052482880812</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1">
-        <v>26662.816505869818</v>
+        <v>26601.939385941761</v>
       </c>
       <c r="B81">
-        <v>130.29737106737537</v>
+        <v>129.1136330986927</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1">
-        <v>26693.236806349767</v>
+        <v>26632.396205389872</v>
       </c>
       <c r="B82">
-        <v>130.19585308624238</v>
+        <v>129.93726954939424</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1">
-        <v>26723.657106829713</v>
+        <v>26662.816505869818</v>
       </c>
       <c r="B83">
-        <v>129.88746827563091</v>
+        <v>130.29737106737537</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1">
-        <v>26754.077407309662</v>
+        <v>26693.236806349767</v>
       </c>
       <c r="B84">
-        <v>129.62888473878274</v>
+        <v>130.19585308624238</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1">
-        <v>26784.534226757769</v>
+        <v>26723.657106829713</v>
       </c>
       <c r="B85">
-        <v>128.90868170282045</v>
+        <v>129.88746827563091</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1">
-        <v>26814.954527237715</v>
+        <v>26754.077407309662</v>
       </c>
       <c r="B86">
-        <v>128.54858018483935</v>
+        <v>129.62888473878274</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1">
-        <v>26845.374827717664</v>
+        <v>26784.534226757769</v>
       </c>
       <c r="B87">
-        <v>129.57716803141312</v>
+        <v>128.90868170282045</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1">
-        <v>26875.795128197609</v>
+        <v>26814.954527237715</v>
       </c>
       <c r="B88">
-        <v>129.73231815352199</v>
+        <v>128.54858018483935</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1">
-        <v>26906.215428677555</v>
+        <v>26845.374827717664</v>
       </c>
       <c r="B89">
-        <v>129.93726954939424</v>
+        <v>129.57716803141312</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1">
-        <v>26936.672248125666</v>
+        <v>26875.795128197609</v>
       </c>
       <c r="B90">
-        <v>130.81262270746538</v>
+        <v>129.73231815352199</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="1">
-        <v>26967.05602963745</v>
+        <v>26906.215428677555</v>
       </c>
       <c r="B91">
-        <v>130.09241967150314</v>
+        <v>129.93726954939424</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1">
-        <v>26997.51284908556</v>
+        <v>26936.672248125666</v>
       </c>
       <c r="B92">
-        <v>129.47373461667382</v>
+        <v>130.81262270746538</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1">
-        <v>27027.933149565506</v>
+        <v>26967.05602963745</v>
       </c>
       <c r="B93">
-        <v>129.1136330986927</v>
+        <v>130.09241967150314</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1">
-        <v>27058.353450045455</v>
+        <v>26997.51284908556</v>
       </c>
       <c r="B94">
-        <v>130.04070296413352</v>
+        <v>129.47373461667382</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1">
-        <v>27088.773750525401</v>
+        <v>27027.933149565506</v>
       </c>
       <c r="B95">
-        <v>132.97514724895848</v>
+        <v>129.1136330986927</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1">
-        <v>27120.180063145755</v>
+        <v>27058.353450045455</v>
       </c>
       <c r="B96">
-        <v>134.10908394387781</v>
+        <v>130.04070296413352</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1">
-        <v>27150.600363625701</v>
+        <v>27088.773750525401</v>
       </c>
       <c r="B97">
-        <v>134.57070344299188</v>
+        <v>132.97514724895848</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1">
-        <v>27181.02066410565</v>
+        <v>27120.180063145755</v>
       </c>
       <c r="B98">
-        <v>134.46727002825264</v>
+        <v>134.10908394387781</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1">
-        <v>27211.440964585596</v>
+        <v>27150.600363625701</v>
       </c>
       <c r="B99">
-        <v>135.8061581190442</v>
+        <v>134.57070344299188</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1">
-        <v>27241.897784033707</v>
+        <v>27181.02066410565</v>
       </c>
       <c r="B100">
-        <v>137.71201455729539</v>
+        <v>134.46727002825264</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1">
-        <v>27272.318084513652</v>
+        <v>27211.440964585596</v>
       </c>
       <c r="B101">
-        <v>139.8726236651822</v>
+        <v>135.8061581190442</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1">
-        <v>27302.738384993598</v>
+        <v>27241.897784033707</v>
       </c>
       <c r="B102">
-        <v>135.54949001580232</v>
+        <v>137.71201455729539</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1">
-        <v>27333.158685473543</v>
+        <v>27272.318084513652</v>
       </c>
       <c r="B103">
-        <v>138.58736771536655</v>
+        <v>139.8726236651822</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1">
-        <v>27363.578985953493</v>
+        <v>27302.738384993598</v>
       </c>
       <c r="B104">
-        <v>137.96868266053727</v>
+        <v>135.54949001580232</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1">
-        <v>27393.999286433438</v>
+        <v>27333.158685473543</v>
       </c>
       <c r="B105">
-        <v>138.22535076377915</v>
+        <v>138.58736771536655</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1">
-        <v>27424.419586913384</v>
+        <v>27363.578985953493</v>
       </c>
       <c r="B106">
-        <v>138.94555379974139</v>
+        <v>137.96868266053727</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1">
-        <v>27454.839887393333</v>
+        <v>27393.999286433438</v>
       </c>
       <c r="B107">
-        <v>139.30757075132883</v>
+        <v>138.22535076377915</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1">
-        <v>27485.296706841444</v>
+        <v>27424.419586913384</v>
       </c>
       <c r="B108">
-        <v>141.10807834123449</v>
+        <v>138.94555379974139</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1">
-        <v>27515.717007321389</v>
+        <v>27454.839887393333</v>
       </c>
       <c r="B109">
-        <v>141.72676339606377</v>
+        <v>139.30757075132883</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1">
-        <v>27546.137307801335</v>
+        <v>27485.296706841444</v>
       </c>
       <c r="B110">
-        <v>143.83757123018722</v>
+        <v>141.10807834123449</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1">
-        <v>27576.557608281284</v>
+        <v>27515.717007321389</v>
       </c>
       <c r="B111">
-        <v>146.72029880764256</v>
+        <v>141.72676339606377</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1">
-        <v>27607.014427729395</v>
+        <v>27546.137307801335</v>
       </c>
       <c r="B112">
-        <v>145.38141071685101</v>
+        <v>143.83757123018722</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1">
-        <v>27637.43472820934</v>
+        <v>27576.557608281284</v>
       </c>
       <c r="B113">
-        <v>148.67595651965712</v>
+        <v>146.72029880764256</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1">
-        <v>27667.855028689286</v>
+        <v>27607.014427729395</v>
       </c>
       <c r="B114">
-        <v>142.34353301728677</v>
+        <v>145.38141071685101</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1">
-        <v>27698.275329169235</v>
+        <v>27637.43472820934</v>
       </c>
       <c r="B115">
-        <v>141.82828137719676</v>
+        <v>148.67595651965712</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1">
-        <v>27728.695629649181</v>
+        <v>27667.855028689286</v>
       </c>
       <c r="B116">
-        <v>139.40908873246178</v>
+        <v>142.34353301728677</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1">
-        <v>27759.152449097292</v>
+        <v>27698.275329169235</v>
       </c>
       <c r="B117">
-        <v>140.95484365273188</v>
+        <v>141.82828137719676</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1">
-        <v>27789.572749577237</v>
+        <v>27728.695629649181</v>
       </c>
       <c r="B118">
-        <v>139.82282239141884</v>
+        <v>139.40908873246178</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1">
-        <v>27819.993050057183</v>
+        <v>27759.152449097292</v>
       </c>
       <c r="B119">
-        <v>137.4017143130776</v>
+        <v>140.95484365273188</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1">
-        <v>27850.413350537132</v>
+        <v>27789.572749577237</v>
       </c>
       <c r="B120">
-        <v>139.5642388545707</v>
+        <v>139.82282239141884</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1">
-        <v>27880.833651017078</v>
+        <v>27819.993050057183</v>
       </c>
       <c r="B121">
-        <v>138.12383278264616</v>
+        <v>137.4017143130776</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1">
-        <v>27911.253951497023</v>
+        <v>27850.413350537132</v>
       </c>
       <c r="B122">
-        <v>139.15242062921993</v>
+        <v>139.5642388545707</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1">
-        <v>27941.710770945134</v>
+        <v>27880.833651017078</v>
       </c>
       <c r="B123">
-        <v>141.05827706747112</v>
+        <v>138.12383278264616</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1">
-        <v>27972.131071425079</v>
+        <v>27911.253951497023</v>
       </c>
       <c r="B124">
-        <v>142.91050136474644</v>
+        <v>139.15242062921993</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1">
-        <v>28002.551371905029</v>
+        <v>27941.710770945134</v>
       </c>
       <c r="B125">
-        <v>142.39524972465642</v>
+        <v>141.05827706747112</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1">
-        <v>28032.971672384974</v>
+        <v>27972.131071425079</v>
       </c>
       <c r="B126">
-        <v>140.90312694536226</v>
+        <v>142.91050136474644</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1">
-        <v>28063.39197286492</v>
+        <v>28002.551371905029</v>
       </c>
       <c r="B127">
-        <v>143.06565148685533</v>
+        <v>142.39524972465642</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1">
-        <v>28093.848792313031</v>
+        <v>28032.971672384974</v>
       </c>
       <c r="B128">
-        <v>146.15524589378919</v>
+        <v>140.90312694536226</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1">
-        <v>28124.232573824818</v>
+        <v>28063.39197286492</v>
       </c>
       <c r="B129">
-        <v>147.23555044773258</v>
+        <v>143.06565148685533</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1">
-        <v>28154.689393272925</v>
+        <v>28093.848792313031</v>
       </c>
       <c r="B130">
-        <v>155.57534836948713</v>
+        <v>146.15524589378919</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1">
-        <v>28185.109693752871</v>
+        <v>28124.232573824818</v>
       </c>
       <c r="B131">
-        <v>153.56605851649667</v>
+        <v>147.23555044773258</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1">
-        <v>28215.52999423282</v>
+        <v>28154.689393272925</v>
       </c>
       <c r="B132">
-        <v>153.41282382799403</v>
+        <v>155.57534836948713</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1">
-        <v>28245.950294712766</v>
+        <v>28185.109693752871</v>
       </c>
       <c r="B133">
-        <v>151.5088828233491</v>
+        <v>153.56605851649667</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1">
-        <v>28276.370595192711</v>
+        <v>28215.52999423282</v>
       </c>
       <c r="B134">
-        <v>147.74888665421634</v>
+        <v>153.41282382799403</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1">
-        <v>28337.247715120771</v>
+        <v>28245.950294712766</v>
       </c>
       <c r="B135">
-        <v>149.80797778097013</v>
+        <v>151.5088828233491</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1">
-        <v>28367.668015600717</v>
+        <v>28276.370595192711</v>
       </c>
       <c r="B136">
-        <v>151.56059953071875</v>
+        <v>147.74888665421634</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1">
-        <v>28398.088316080662</v>
+        <v>28337.247715120771</v>
       </c>
       <c r="B137">
-        <v>151.66211751185173</v>
+        <v>149.80797778097013</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1">
-        <v>28428.508616560612</v>
+        <v>28367.668015600717</v>
       </c>
       <c r="B138">
-        <v>153.05272231001294</v>
+        <v>151.56059953071875</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1">
-        <v>28458.928917040557</v>
+        <v>28398.088316080662</v>
       </c>
       <c r="B139">
-        <v>155.47191495474789</v>
+        <v>151.66211751185173</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1">
-        <v>28489.349217520503</v>
+        <v>28428.508616560612</v>
       </c>
       <c r="B140">
-        <v>149.39615955561939</v>
+        <v>153.05272231001294</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1">
-        <v>28519.806036968614</v>
+        <v>28458.928917040557</v>
       </c>
       <c r="B141">
-        <v>146.40999856342478</v>
+        <v>155.47191495474789</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1">
-        <v>28550.226337448563</v>
+        <v>28489.349217520503</v>
       </c>
       <c r="B142">
-        <v>107.08040032562371</v>
+        <v>149.39615955561939</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1">
-        <v>28580.646637928508</v>
+        <v>28519.806036968614</v>
       </c>
       <c r="B143">
-        <v>146.25676387492217</v>
+        <v>146.40999856342478</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1">
-        <v>28611.066938408454</v>
+        <v>28550.226337448563</v>
       </c>
       <c r="B144">
-        <v>118.50979265431212</v>
+        <v>107.08040032562371</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1">
-        <v>28641.487238888403</v>
+        <v>28580.646637928508</v>
       </c>
       <c r="B145">
-        <v>143.42383757123019</v>
+        <v>146.25676387492217</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1">
-        <v>28671.907539368349</v>
+        <v>28611.066938408454</v>
       </c>
       <c r="B146">
-        <v>141.15979504860411</v>
+        <v>118.50979265431212</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1">
-        <v>28702.327839848294</v>
+        <v>28641.487238888403</v>
       </c>
       <c r="B147">
-        <v>141.05827706747112</v>
+        <v>143.42383757123019</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1">
-        <v>28732.784659296405</v>
+        <v>28671.907539368349</v>
       </c>
       <c r="B148">
-        <v>144.96959249150024</v>
+        <v>141.15979504860411</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1">
-        <v>28763.204959776351</v>
+        <v>28702.327839848294</v>
       </c>
       <c r="B149">
-        <v>138.89575252597808</v>
+        <v>141.05827706747112</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1">
-        <v>28793.625260256296</v>
+        <v>28732.784659296405</v>
       </c>
       <c r="B150">
-        <v>137.09332950246613</v>
+        <v>144.96959249150024</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1">
-        <v>28824.045560736246</v>
+        <v>28763.204959776351</v>
       </c>
       <c r="B151">
-        <v>135.54949001580232</v>
+        <v>138.89575252597808</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1">
-        <v>28854.465861216191</v>
+        <v>28793.625260256296</v>
       </c>
       <c r="B152">
-        <v>137.14504620983575</v>
+        <v>137.09332950246613</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1">
-        <v>28884.922680664302</v>
+        <v>28824.045560736246</v>
       </c>
       <c r="B153">
-        <v>136.83666139922423</v>
+        <v>135.54949001580232</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1">
-        <v>28915.342981144247</v>
+        <v>28854.465861216191</v>
       </c>
       <c r="B154">
-        <v>135.85787482641382</v>
+        <v>137.14504620983575</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1">
-        <v>28945.763281624197</v>
+        <v>28884.922680664302</v>
       </c>
       <c r="B155">
-        <v>134.41746875448928</v>
+        <v>136.83666139922423</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1">
-        <v>28976.183582104142</v>
+        <v>28915.342981144247</v>
       </c>
       <c r="B156">
-        <v>134.87908825360341</v>
+        <v>135.85787482641382</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1">
-        <v>29006.603882584088</v>
+        <v>28945.763281624197</v>
       </c>
       <c r="B157">
-        <v>134.26231863238041</v>
+        <v>134.41746875448928</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1">
-        <v>29037.024183064037</v>
+        <v>28976.183582104142</v>
       </c>
       <c r="B158">
-        <v>134.62242015036153</v>
+        <v>134.87908825360341</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1">
-        <v>29067.444483543983</v>
+        <v>29006.603882584088</v>
       </c>
       <c r="B159">
-        <v>135.54949001580232</v>
+        <v>134.26231863238041</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1">
-        <v>29097.901302992093</v>
+        <v>29037.024183064037</v>
       </c>
       <c r="B160">
-        <v>135.29282191256044</v>
+        <v>134.62242015036153</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1">
-        <v>29128.321603472039</v>
+        <v>29067.444483543983</v>
       </c>
       <c r="B161">
-        <v>135.75444141167458</v>
+        <v>135.54949001580232</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1">
-        <v>29189.162204431934</v>
+        <v>29097.901302992093</v>
       </c>
       <c r="B162">
-        <v>135.85787482641382</v>
+        <v>135.29282191256044</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1">
-        <v>29219.582504911879</v>
+        <v>29128.321603472039</v>
       </c>
       <c r="B163">
-        <v>133.90221711439926</v>
+        <v>135.75444141167458</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1">
-        <v>29250.002805391829</v>
+        <v>29189.162204431934</v>
       </c>
       <c r="B164">
-        <v>131.79140928027581</v>
+        <v>135.85787482641382</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1">
-        <v>29280.386586903609</v>
+        <v>29219.582504911879</v>
       </c>
       <c r="B165">
-        <v>135.24110520519082</v>
+        <v>133.90221711439926</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1">
-        <v>29310.879925319885</v>
+        <v>29250.002805391829</v>
       </c>
       <c r="B166">
-        <v>132.87171383421921</v>
+        <v>131.79140928027581</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1">
-        <v>29341.263706831669</v>
+        <v>29280.386586903609</v>
       </c>
       <c r="B167">
-        <v>134.72585356510081</v>
+        <v>135.24110520519082</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1">
-        <v>29371.684007311615</v>
+        <v>29310.879925319885</v>
       </c>
       <c r="B168">
-        <v>134.26231863238041</v>
+        <v>132.87171383421921</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1">
-        <v>29402.10430779156</v>
+        <v>29341.263706831669</v>
       </c>
       <c r="B169">
-        <v>135.65100799693528</v>
+        <v>134.72585356510081</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1">
-        <v>29432.524608271509</v>
+        <v>29371.684007311615</v>
       </c>
       <c r="B170">
-        <v>133.95393382176889</v>
+        <v>134.26231863238041</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1">
-        <v>29462.944908751455</v>
+        <v>29402.10430779156</v>
       </c>
       <c r="B171">
-        <v>131.12292295168317</v>
+        <v>135.65100799693528</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1">
-        <v>29493.365209231401</v>
+        <v>29432.524608271509</v>
       </c>
       <c r="B172">
-        <v>134.3638366135134</v>
+        <v>133.95393382176889</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1">
-        <v>29523.822028679511</v>
+        <v>29462.944908751455</v>
       </c>
       <c r="B173">
-        <v>134.82928697984005</v>
+        <v>131.12292295168317</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1">
-        <v>29554.24232915946</v>
+        <v>29493.365209231401</v>
       </c>
       <c r="B174">
-        <v>136.37312646650383</v>
+        <v>134.3638366135134</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1">
-        <v>29584.662629639406</v>
+        <v>29523.822028679511</v>
       </c>
       <c r="B175">
-        <v>134.72585356510081</v>
+        <v>134.82928697984005</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1">
-        <v>29615.082930119352</v>
+        <v>29554.24232915946</v>
       </c>
       <c r="B176">
-        <v>135.08595508308193</v>
+        <v>136.37312646650383</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="1">
-        <v>29645.503230599301</v>
+        <v>29584.662629639406</v>
       </c>
       <c r="B177">
-        <v>141.67504668869415</v>
+        <v>134.72585356510081</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="1">
-        <v>29675.960050047408</v>
+        <v>29615.082930119352</v>
       </c>
       <c r="B178">
-        <v>142.39524972465642</v>
+        <v>135.08595508308193</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="1">
-        <v>29706.380350527357</v>
+        <v>29645.503230599301</v>
       </c>
       <c r="B179">
-        <v>140.74797682325334</v>
+        <v>141.67504668869415</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="1">
-        <v>29736.800651007303</v>
+        <v>29675.960050047408</v>
       </c>
       <c r="B180">
         <v>142.39524972465642</v>
@@ -43852,999 +43860,999 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="1">
-        <v>29767.220951487248</v>
+        <v>29706.380350527357</v>
       </c>
       <c r="B181">
-        <v>140.0277737872911</v>
+        <v>140.74797682325334</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="1">
-        <v>29797.641251967194</v>
+        <v>29736.800651007303</v>
       </c>
       <c r="B182">
-        <v>138.89575252597808</v>
+        <v>142.39524972465642</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="1">
-        <v>29828.061552447143</v>
+        <v>29767.220951487248</v>
       </c>
       <c r="B183">
-        <v>137.66029784992577</v>
+        <v>140.0277737872911</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="1">
-        <v>29858.518371895254</v>
+        <v>29797.641251967194</v>
       </c>
       <c r="B184">
-        <v>138.12383278264616</v>
+        <v>138.89575252597808</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="1">
-        <v>29888.9386723752</v>
+        <v>29828.061552447143</v>
       </c>
       <c r="B185">
-        <v>135.8061581190442</v>
+        <v>137.66029784992577</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="1">
-        <v>29919.358972855145</v>
+        <v>29858.518371895254</v>
       </c>
       <c r="B186">
-        <v>134.82928697984005</v>
+        <v>138.12383278264616</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="1">
-        <v>29949.779273335094</v>
+        <v>29888.9386723752</v>
       </c>
       <c r="B187">
-        <v>136.62979456974574</v>
+        <v>135.8061581190442</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="1">
-        <v>29949.815792303256</v>
+        <v>29919.358972855145</v>
       </c>
       <c r="B188">
-        <v>136.62979456974574</v>
+        <v>134.82928697984005</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="1">
-        <v>29980.236092783205</v>
+        <v>29949.779273335094</v>
       </c>
       <c r="B189">
-        <v>135.60120672317194</v>
+        <v>136.62979456974574</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="1">
-        <v>30010.656393263151</v>
+        <v>29949.815792303256</v>
       </c>
       <c r="B190">
-        <v>129.1136330986927</v>
+        <v>136.62979456974574</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="1">
-        <v>30041.076693743096</v>
+        <v>29980.236092783205</v>
       </c>
       <c r="B191">
-        <v>130.29737106737537</v>
+        <v>135.60120672317194</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="1">
-        <v>30071.496994223045</v>
+        <v>30010.656393263151</v>
       </c>
       <c r="B192">
-        <v>129.88746827563091</v>
+        <v>129.1136330986927</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="1">
-        <v>30102.903306843396</v>
+        <v>30041.076693743096</v>
       </c>
       <c r="B193">
-        <v>129.01211511755974</v>
+        <v>130.29737106737537</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="1">
-        <v>30133.360126291507</v>
+        <v>30071.496994223045</v>
       </c>
       <c r="B194">
-        <v>128.34171335536081</v>
+        <v>129.88746827563091</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="1">
-        <v>30163.780426771453</v>
+        <v>30102.903306843396</v>
       </c>
       <c r="B195">
-        <v>127.98161183737969</v>
+        <v>129.01211511755974</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="1">
-        <v>30194.200727251402</v>
+        <v>30133.360126291507</v>
       </c>
       <c r="B196">
-        <v>127.41655892352631</v>
+        <v>128.34171335536081</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="1">
-        <v>30224.621027731348</v>
+        <v>30163.780426771453</v>
       </c>
       <c r="B197">
-        <v>127.56979361202892</v>
+        <v>127.98161183737969</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="1">
-        <v>30255.041328211293</v>
+        <v>30194.200727251402</v>
       </c>
       <c r="B198">
-        <v>127.20969209404778</v>
+        <v>127.41655892352631</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="1">
-        <v>30285.498147659404</v>
+        <v>30224.621027731348</v>
       </c>
       <c r="B199">
-        <v>127.15797538667816</v>
+        <v>127.56979361202892</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1">
-        <v>30315.881929171188</v>
+        <v>30255.041328211293</v>
       </c>
       <c r="B200">
-        <v>127.15797538667816</v>
+        <v>127.20969209404778</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="1">
-        <v>30346.338748619299</v>
+        <v>30285.498147659404</v>
       </c>
       <c r="B201">
-        <v>126.79787386869702</v>
+        <v>127.15797538667816</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1">
-        <v>30376.759049099244</v>
+        <v>30315.881929171188</v>
       </c>
       <c r="B202">
-        <v>127.31312550878704</v>
+        <v>127.15797538667816</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="1">
-        <v>30407.179349579194</v>
+        <v>30346.338748619299</v>
       </c>
       <c r="B203">
-        <v>129.21706651343197</v>
+        <v>126.79787386869702</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="1">
-        <v>30437.599650059139</v>
+        <v>30376.759049099244</v>
       </c>
       <c r="B204">
-        <v>131.63625915816692</v>
+        <v>127.31312550878704</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="1">
-        <v>30468.019950539085</v>
+        <v>30407.179349579194</v>
       </c>
       <c r="B205">
-        <v>132.45989560886846</v>
+        <v>129.21706651343197</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="1">
-        <v>30498.476769987195</v>
+        <v>30437.599650059139</v>
       </c>
       <c r="B206">
-        <v>131.99636067614807</v>
+        <v>131.63625915816692</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="1">
-        <v>30528.860551498979</v>
+        <v>30468.019950539085</v>
       </c>
       <c r="B207">
-        <v>131.73969257290616</v>
+        <v>132.45989560886846</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1">
-        <v>30559.317370947087</v>
+        <v>30498.476769987195</v>
       </c>
       <c r="B208">
-        <v>130.65747258535652</v>
+        <v>131.99636067614807</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="1">
-        <v>30589.737671427036</v>
+        <v>30528.860551498979</v>
       </c>
       <c r="B209">
-        <v>129.83575156826126</v>
+        <v>131.73969257290616</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="1">
-        <v>30620.157971906985</v>
+        <v>30559.317370947087</v>
       </c>
       <c r="B210">
-        <v>128.08504525211893</v>
+        <v>130.65747258535652</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="1">
-        <v>30650.578272386931</v>
+        <v>30589.737671427036</v>
       </c>
       <c r="B211">
-        <v>128.70181487334196</v>
+        <v>129.83575156826126</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="1">
-        <v>30680.998572866876</v>
+        <v>30620.157971906985</v>
       </c>
       <c r="B212">
-        <v>131.12292295168317</v>
+        <v>128.08504525211893</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="1">
-        <v>30711.455392314987</v>
+        <v>30650.578272386931</v>
       </c>
       <c r="B213">
-        <v>112.33251927405065</v>
+        <v>128.70181487334196</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="1">
-        <v>30741.875692794936</v>
+        <v>30680.998572866876</v>
       </c>
       <c r="B214">
-        <v>131.73969257290616</v>
+        <v>131.12292295168317</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="1">
-        <v>30772.295993274882</v>
+        <v>30711.455392314987</v>
       </c>
       <c r="B215">
-        <v>131.79140928027581</v>
+        <v>112.33251927405065</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="1">
-        <v>30802.716293754827</v>
+        <v>30741.875692794936</v>
       </c>
       <c r="B216">
-        <v>131.01948953694392</v>
+        <v>131.73969257290616</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="1">
-        <v>30833.136594234777</v>
+        <v>30772.295993274882</v>
       </c>
       <c r="B217">
-        <v>129.78403486089161</v>
+        <v>131.79140928027581</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="1">
-        <v>30863.556894714722</v>
+        <v>30802.716293754827</v>
       </c>
       <c r="B218">
-        <v>127.31312550878704</v>
+        <v>131.01948953694392</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="1">
-        <v>30893.977195194668</v>
+        <v>30833.136594234777</v>
       </c>
       <c r="B219">
-        <v>126.64272374658812</v>
+        <v>129.78403486089161</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="1">
-        <v>30924.434014642778</v>
+        <v>30863.556894714722</v>
       </c>
       <c r="B220">
-        <v>126.79787386869702</v>
+        <v>127.31312550878704</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="1">
-        <v>30954.854315122728</v>
+        <v>30893.977195194668</v>
       </c>
       <c r="B221">
-        <v>126.282622228607</v>
+        <v>126.64272374658812</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="1">
-        <v>30985.27461560267</v>
+        <v>30924.434014642778</v>
       </c>
       <c r="B222">
-        <v>126.12938754010437</v>
+        <v>126.79787386869702</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="1">
-        <v>31015.694916082619</v>
+        <v>30954.854315122728</v>
       </c>
       <c r="B223">
-        <v>126.18110424747401</v>
+        <v>126.282622228607</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1">
-        <v>31046.115216562564</v>
+        <v>30985.27461560267</v>
       </c>
       <c r="B224">
-        <v>125.56241919264473</v>
+        <v>126.12938754010437</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1">
-        <v>31076.498998074348</v>
+        <v>31015.694916082619</v>
       </c>
       <c r="B225">
-        <v>125.45898577790547</v>
+        <v>126.18110424747401</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1">
-        <v>31106.955817522459</v>
+        <v>31046.115216562564</v>
       </c>
       <c r="B226">
-        <v>125.45898577790547</v>
+        <v>125.56241919264473</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="1">
-        <v>31137.41263697057</v>
+        <v>31076.498998074348</v>
       </c>
       <c r="B227">
-        <v>125.25403438203323</v>
+        <v>125.45898577790547</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1">
-        <v>31167.79641848235</v>
+        <v>31106.955817522459</v>
       </c>
       <c r="B228">
-        <v>124.22353110185317</v>
+        <v>125.45898577790547</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="1">
-        <v>31198.253237930461</v>
+        <v>31137.41263697057</v>
       </c>
       <c r="B229">
-        <v>124.48211463870132</v>
+        <v>125.25403438203323</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1">
-        <v>31228.637019442245</v>
+        <v>31167.79641848235</v>
       </c>
       <c r="B230">
-        <v>124.99545084518506</v>
+        <v>124.22353110185317</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="1">
-        <v>31259.093838890356</v>
+        <v>31198.253237930461</v>
       </c>
       <c r="B231">
-        <v>124.99545084518506</v>
+        <v>124.48211463870132</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1">
-        <v>31289.550658338467</v>
+        <v>31228.637019442245</v>
       </c>
       <c r="B232">
-        <v>124.32696451659244</v>
+        <v>124.99545084518506</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="1">
-        <v>31319.934439850251</v>
+        <v>31259.093838890356</v>
       </c>
       <c r="B233">
-        <v>124.89393286405209</v>
+        <v>124.99545084518506</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1">
-        <v>31350.391259298362</v>
+        <v>31289.550658338467</v>
       </c>
       <c r="B234">
-        <v>124.99545084518506</v>
+        <v>124.32696451659244</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1">
-        <v>31380.775040810142</v>
+        <v>31319.934439850251</v>
       </c>
       <c r="B235">
-        <v>127.6713115931619</v>
+        <v>124.89393286405209</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1">
-        <v>31411.195341290091</v>
+        <v>31350.391259298362</v>
       </c>
       <c r="B236">
-        <v>127.56979361202892</v>
+        <v>124.99545084518506</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="1">
-        <v>31441.615641770037</v>
+        <v>31380.775040810142</v>
       </c>
       <c r="B237">
-        <v>127.56979361202892</v>
+        <v>127.6713115931619</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1">
-        <v>31472.072461218148</v>
+        <v>31411.195341290091</v>
       </c>
       <c r="B238">
-        <v>126.95110855719963</v>
+        <v>127.56979361202892</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="1">
-        <v>31502.492761698093</v>
+        <v>31441.615641770037</v>
       </c>
       <c r="B239">
-        <v>126.38605564334625</v>
+        <v>127.56979361202892</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1">
-        <v>31532.913062178042</v>
+        <v>31472.072461218148</v>
       </c>
       <c r="B240">
-        <v>126.54120576545515</v>
+        <v>126.95110855719963</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1">
-        <v>31563.333362657988</v>
+        <v>31502.492761698093</v>
       </c>
       <c r="B241">
-        <v>125.71756931475362</v>
+        <v>126.38605564334625</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1">
-        <v>31593.790182106095</v>
+        <v>31532.913062178042</v>
       </c>
       <c r="B242">
-        <v>124.68706603457356</v>
+        <v>126.54120576545515</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1">
-        <v>31624.210482586044</v>
+        <v>31563.333362657988</v>
       </c>
       <c r="B243">
-        <v>124.42848249772541</v>
+        <v>125.71756931475362</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="1">
-        <v>31685.087602514101</v>
+        <v>31593.790182106095</v>
       </c>
       <c r="B244">
-        <v>124.32696451659244</v>
+        <v>124.68706603457356</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="1">
-        <v>31715.507902994046</v>
+        <v>31624.210482586044</v>
       </c>
       <c r="B245">
-        <v>124.12009768711391</v>
+        <v>124.42848249772541</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1">
-        <v>31745.928203473995</v>
+        <v>31685.087602514101</v>
       </c>
       <c r="B246">
-        <v>121.64918833500933</v>
+        <v>124.32696451659244</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1">
-        <v>31776.348503953945</v>
+        <v>31715.507902994046</v>
       </c>
       <c r="B247">
-        <v>121.90777187185749</v>
+        <v>124.12009768711391</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1">
-        <v>31806.768804433887</v>
+        <v>31745.928203473995</v>
       </c>
       <c r="B248">
-        <v>121.34080352439783</v>
+        <v>121.64918833500933</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1">
-        <v>31837.189104913836</v>
+        <v>31776.348503953945</v>
       </c>
       <c r="B249">
-        <v>121.23737010965857</v>
+        <v>121.90777187185749</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="1">
-        <v>31867.609405393781</v>
+        <v>31806.768804433887</v>
       </c>
       <c r="B250">
-        <v>121.44423693913708</v>
+        <v>121.34080352439783</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="1">
-        <v>31898.066224841892</v>
+        <v>31837.189104913836</v>
       </c>
       <c r="B251">
-        <v>120.98070200641671</v>
+        <v>121.23737010965857</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="1">
-        <v>31928.523044289999</v>
+        <v>31867.609405393781</v>
       </c>
       <c r="B252">
-        <v>120.77575061054446</v>
+        <v>121.44423693913708</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="1">
-        <v>31958.906825801787</v>
+        <v>31898.066224841892</v>
       </c>
       <c r="B253">
-        <v>120.46545036632668</v>
+        <v>120.98070200641671</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="1">
-        <v>31989.363645249898</v>
+        <v>31928.523044289999</v>
       </c>
       <c r="B254">
-        <v>120.00191543360627</v>
+        <v>120.77575061054446</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="1">
-        <v>32019.820464698005</v>
+        <v>31958.906825801787</v>
       </c>
       <c r="B255">
-        <v>119.79696403773403</v>
+        <v>120.46545036632668</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="1">
-        <v>32050.204246209789</v>
+        <v>31989.363645249898</v>
       </c>
       <c r="B256">
-        <v>120.46545036632668</v>
+        <v>120.00191543360627</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="1">
-        <v>32080.6610656579</v>
+        <v>32019.820464698005</v>
       </c>
       <c r="B257">
-        <v>120.67231719580519</v>
+        <v>119.79696403773403</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="1">
-        <v>32111.04484716968</v>
+        <v>32050.204246209789</v>
       </c>
       <c r="B258">
-        <v>121.1339366949193</v>
+        <v>120.46545036632668</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1">
-        <v>32141.501666617791</v>
+        <v>32080.6610656579</v>
       </c>
       <c r="B259">
-        <v>120.62060048843556</v>
+        <v>120.67231719580519</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="1">
-        <v>32171.885448129578</v>
+        <v>32111.04484716968</v>
       </c>
       <c r="B260">
-        <v>120.5171670736963</v>
+        <v>121.1339366949193</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="1">
-        <v>32202.342267577686</v>
+        <v>32141.501666617791</v>
       </c>
       <c r="B261">
-        <v>120.00191543360627</v>
+        <v>120.62060048843556</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="1">
-        <v>32232.72604908947</v>
+        <v>32171.885448129578</v>
       </c>
       <c r="B262">
-        <v>120.56888378106594</v>
+        <v>120.5171670736963</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="1">
-        <v>32263.18286853758</v>
+        <v>32202.342267577686</v>
       </c>
       <c r="B263">
-        <v>120.72211846956856</v>
+        <v>120.00191543360627</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="1">
-        <v>32293.566650049364</v>
+        <v>32232.72604908947</v>
       </c>
       <c r="B264">
-        <v>119.79696403773403</v>
+        <v>120.56888378106594</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="1">
-        <v>32324.023469497475</v>
+        <v>32263.18286853758</v>
       </c>
       <c r="B265">
-        <v>120.46545036632668</v>
+        <v>120.72211846956856</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="1">
-        <v>32354.480288945582</v>
+        <v>32293.566650049364</v>
       </c>
       <c r="B266">
-        <v>120.10534884834554</v>
+        <v>119.79696403773403</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="1">
-        <v>32384.86407045737</v>
+        <v>32324.023469497475</v>
       </c>
       <c r="B267">
-        <v>120.31030024421779</v>
+        <v>120.46545036632668</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="1">
-        <v>32415.320889905481</v>
+        <v>32354.480288945582</v>
       </c>
       <c r="B268">
-        <v>116.39898482018866</v>
+        <v>120.10534884834554</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="1">
-        <v>32445.777709353588</v>
+        <v>32384.86407045737</v>
       </c>
       <c r="B269">
-        <v>119.28171239764401</v>
+        <v>120.31030024421779</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="1">
-        <v>32476.161490865372</v>
+        <v>32415.320889905481</v>
       </c>
       <c r="B270">
-        <v>118.86989417229324</v>
+        <v>116.39898482018866</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="1">
-        <v>32506.618310313483</v>
+        <v>32445.777709353588</v>
       </c>
       <c r="B271">
-        <v>118.50979265431212</v>
+        <v>119.28171239764401</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="1">
-        <v>32537.002091825267</v>
+        <v>32476.161490865372</v>
       </c>
       <c r="B272">
-        <v>120.00191543360627</v>
+        <v>118.86989417229324</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="1">
-        <v>32567.458911273374</v>
+        <v>32506.618310313483</v>
       </c>
       <c r="B273">
-        <v>119.69353062299477</v>
+        <v>118.50979265431212</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="1">
-        <v>32597.842692785161</v>
+        <v>32537.002091825267</v>
       </c>
       <c r="B274">
-        <v>118.45807594694249</v>
+        <v>120.00191543360627</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="1">
-        <v>32628.299512233272</v>
+        <v>32567.458911273374</v>
       </c>
       <c r="B275">
-        <v>117.37777139299909</v>
+        <v>119.69353062299477</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="1">
-        <v>32658.756331681379</v>
+        <v>32597.842692785161</v>
       </c>
       <c r="B276">
-        <v>117.63443949624096</v>
+        <v>118.45807594694249</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="1">
-        <v>32689.140113193163</v>
+        <v>32628.299512233272</v>
       </c>
       <c r="B277">
-        <v>117.27433797825982</v>
+        <v>117.37777139299909</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="1">
-        <v>32719.523894704947</v>
+        <v>32658.756331681379</v>
       </c>
       <c r="B278">
-        <v>117.06747114878131</v>
+        <v>117.63443949624096</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="1">
-        <v>32749.980714153055</v>
+        <v>32689.140113193163</v>
       </c>
       <c r="B279">
-        <v>116.6039362160609</v>
+        <v>117.27433797825982</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="1">
-        <v>32780.437533601165</v>
+        <v>32719.523894704947</v>
       </c>
       <c r="B280">
-        <v>116.45070152755829</v>
+        <v>117.06747114878131</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" s="1">
-        <v>32810.821315112953</v>
+        <v>32749.980714153055</v>
       </c>
       <c r="B281">
-        <v>116.45070152755829</v>
+        <v>116.6039362160609</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="1">
-        <v>32841.278134561057</v>
+        <v>32780.437533601165</v>
       </c>
       <c r="B282">
-        <v>116.39898482018866</v>
+        <v>116.45070152755829</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="1">
-        <v>32871.734954009167</v>
+        <v>32810.821315112953</v>
       </c>
       <c r="B283">
-        <v>116.50241823492793</v>
+        <v>116.45070152755829</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" s="1">
-        <v>32902.118735520955</v>
+        <v>32841.278134561057</v>
       </c>
       <c r="B284">
-        <v>116.24383469807977</v>
+        <v>116.39898482018866</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" s="1">
-        <v>32932.575554969066</v>
+        <v>32871.734954009167</v>
       </c>
       <c r="B285">
-        <v>115.83393190633528</v>
+        <v>116.50241823492793</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" s="1">
-        <v>32962.959336480846</v>
+        <v>32902.118735520955</v>
       </c>
       <c r="B286">
-        <v>117.17090456352057</v>
+        <v>116.24383469807977</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" s="1">
-        <v>32993.416155928957</v>
+        <v>32932.575554969066</v>
       </c>
       <c r="B287">
-        <v>115.06009672939712</v>
+        <v>115.83393190633528</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" s="1">
-        <v>33023.872975377068</v>
+        <v>32962.959336480846</v>
       </c>
       <c r="B288">
-        <v>114.7517119187856</v>
+        <v>117.17090456352057</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" s="1">
-        <v>33054.256756888848</v>
+        <v>32993.416155928957</v>
       </c>
       <c r="B289">
-        <v>114.1349422975626</v>
+        <v>115.06009672939712</v>
       </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" s="1">
-        <v>33085.626550541041</v>
+        <v>33023.872975377068</v>
       </c>
       <c r="B290">
-        <v>114.23646027869557</v>
+        <v>114.7517119187856</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" s="1">
-        <v>33116.04685102099</v>
+        <v>33054.256756888848</v>
       </c>
       <c r="B291">
-        <v>114.64827850404635</v>
+        <v>114.1349422975626</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" s="1">
-        <v>33146.503670469101</v>
+        <v>33085.626550541041</v>
       </c>
       <c r="B292">
-        <v>115.21524685150601</v>
+        <v>114.23646027869557</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293" s="1">
-        <v>33176.923970949043</v>
+        <v>33116.04685102099</v>
       </c>
       <c r="B293">
-        <v>114.39161040080447</v>
+        <v>114.64827850404635</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294" s="1">
-        <v>33207.344271428992</v>
+        <v>33146.503670469101</v>
       </c>
       <c r="B294">
-        <v>114.1349422975626</v>
+        <v>115.21524685150601</v>
       </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295" s="1">
-        <v>33237.801090877103</v>
+        <v>33176.923970949043</v>
       </c>
       <c r="B295">
-        <v>113.51625724273333</v>
+        <v>114.39161040080447</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" s="1">
-        <v>33268.221391357045</v>
+        <v>33207.344271428992</v>
       </c>
       <c r="B296">
-        <v>114.23646027869557</v>
+        <v>114.1349422975626</v>
       </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" s="1">
-        <v>33298.641691836994</v>
+        <v>33237.801090877103</v>
       </c>
       <c r="B297">
-        <v>114.7517119187856</v>
+        <v>113.51625724273333</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="1">
-        <v>33329.025473348782</v>
+        <v>33268.221391357045</v>
       </c>
       <c r="B298">
-        <v>113.51625724273333</v>
+        <v>114.23646027869557</v>
       </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299" s="1">
-        <v>33359.482292796893</v>
+        <v>33298.641691836994</v>
       </c>
       <c r="B299">
-        <v>113.9797921754537</v>
+        <v>114.7517119187856</v>
       </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" s="1">
-        <v>33389.939112245003</v>
+        <v>33329.025473348782</v>
       </c>
       <c r="B300">
-        <v>113.9261600344778</v>
+        <v>113.51625724273333</v>
       </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301" s="1">
-        <v>33420.322893756784</v>
+        <v>33359.482292796893</v>
       </c>
       <c r="B301">
-        <v>113.67140736484222</v>
+        <v>113.9797921754537</v>
       </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" s="1">
-        <v>33450.779713204895</v>
+        <v>33389.939112245003</v>
       </c>
       <c r="B302">
-        <v>113.4645405353637</v>
+        <v>113.9261600344778</v>
       </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303" s="1">
-        <v>33481.200013684836</v>
+        <v>33420.322893756784</v>
       </c>
       <c r="B303">
-        <v>113.9261600344778</v>
+        <v>113.67140736484222</v>
       </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304" s="1">
-        <v>33511.620314164786</v>
+        <v>33450.779713204895</v>
       </c>
       <c r="B304">
-        <v>113.72312407221186</v>
+        <v>113.4645405353637</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305" s="1">
-        <v>33542.040614644735</v>
+        <v>33481.200013684836</v>
       </c>
       <c r="B305">
         <v>113.9261600344778</v>
@@ -44852,855 +44860,855 @@
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="1">
-        <v>33572.497434092846</v>
+        <v>33511.620314164786</v>
       </c>
       <c r="B306">
-        <v>114.69999521141598</v>
+        <v>113.72312407221186</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="1">
-        <v>33602.917734572788</v>
+        <v>33542.040614644735</v>
       </c>
       <c r="B307">
-        <v>114.69999521141598</v>
+        <v>113.9261600344778</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" s="1">
-        <v>33633.338035052737</v>
+        <v>33572.497434092846</v>
       </c>
       <c r="B308">
-        <v>115.21524685150601</v>
+        <v>114.69999521141598</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309" s="1">
-        <v>33663.758335532686</v>
+        <v>33602.917734572788</v>
       </c>
       <c r="B309">
-        <v>115.47191495474789</v>
+        <v>114.69999521141598</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310" s="1">
-        <v>33694.21515498079</v>
+        <v>33633.338035052737</v>
       </c>
       <c r="B310">
-        <v>117.11918785615094</v>
+        <v>115.21524685150601</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" s="1">
-        <v>33724.635455460739</v>
+        <v>33663.758335532686</v>
       </c>
       <c r="B311">
-        <v>114.80342862615524</v>
+        <v>115.47191495474789</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" s="1">
-        <v>33755.055755940688</v>
+        <v>33694.21515498079</v>
       </c>
       <c r="B312">
-        <v>115.06009672939712</v>
+        <v>117.11918785615094</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313" s="1">
-        <v>33785.439537452468</v>
+        <v>33724.635455460739</v>
       </c>
       <c r="B313">
-        <v>116.24383469807977</v>
+        <v>114.80342862615524</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="1">
-        <v>33815.896356900579</v>
+        <v>33755.055755940688</v>
       </c>
       <c r="B314">
-        <v>116.2955514054494</v>
+        <v>115.06009672939712</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315" s="1">
-        <v>33846.316657380528</v>
+        <v>33785.439537452468</v>
       </c>
       <c r="B315">
-        <v>115.93544988746827</v>
+        <v>116.24383469807977</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" s="1">
-        <v>33876.73695786047</v>
+        <v>33815.896356900579</v>
       </c>
       <c r="B316">
-        <v>116.65756835703682</v>
+        <v>116.2955514054494</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317" s="1">
-        <v>33907.15725834042</v>
+        <v>33846.316657380528</v>
       </c>
       <c r="B317">
-        <v>117.11918785615094</v>
+        <v>115.93544988746827</v>
       </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318" s="1">
-        <v>33937.61407778853</v>
+        <v>33876.73695786047</v>
       </c>
       <c r="B318">
-        <v>117.37777139299909</v>
+        <v>116.65756835703682</v>
       </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319" s="1">
-        <v>33968.070897236641</v>
+        <v>33907.15725834042</v>
       </c>
       <c r="B319">
-        <v>116.75908633816979</v>
+        <v>117.11918785615094</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" s="1">
-        <v>33998.454678748429</v>
+        <v>33937.61407778853</v>
       </c>
       <c r="B320">
-        <v>116.75908633816979</v>
+        <v>117.37777139299909</v>
       </c>
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="1">
-        <v>34028.911498196539</v>
+        <v>33968.070897236641</v>
       </c>
       <c r="B321">
-        <v>116.6039362160609</v>
+        <v>116.75908633816979</v>
       </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322" s="1">
-        <v>34059.29527970832</v>
+        <v>33998.454678748429</v>
       </c>
       <c r="B322">
-        <v>117.8393908921132</v>
+        <v>116.75908633816979</v>
       </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323" s="1">
-        <v>34089.752099156431</v>
+        <v>34028.911498196539</v>
       </c>
       <c r="B323">
-        <v>116.9142364602787</v>
+        <v>116.6039362160609</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" s="1">
-        <v>34120.135880668211</v>
+        <v>34059.29527970832</v>
       </c>
       <c r="B324">
-        <v>115.00838002202748</v>
+        <v>117.8393908921132</v>
       </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325" s="1">
-        <v>34150.592700116322</v>
+        <v>34089.752099156431</v>
       </c>
       <c r="B325">
-        <v>115.00838002202748</v>
+        <v>116.9142364602787</v>
       </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326" s="1">
-        <v>34181.049519564433</v>
+        <v>34120.135880668211</v>
       </c>
       <c r="B326">
-        <v>115.57534836948714</v>
+        <v>115.00838002202748</v>
       </c>
     </row>
     <row r="327" spans="1:2">
       <c r="A327" s="1">
-        <v>34211.43330107622</v>
+        <v>34150.592700116322</v>
       </c>
       <c r="B327">
-        <v>116.34726811281902</v>
+        <v>115.00838002202748</v>
       </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="1">
-        <v>34241.890120524331</v>
+        <v>34181.049519564433</v>
       </c>
       <c r="B328">
-        <v>115.67878178422639</v>
+        <v>115.57534836948714</v>
       </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329" s="1">
-        <v>34272.346939972434</v>
+        <v>34211.43330107622</v>
       </c>
       <c r="B329">
-        <v>115.67878178422639</v>
+        <v>116.34726811281902</v>
       </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="1">
-        <v>34302.730721484222</v>
+        <v>34241.890120524331</v>
       </c>
       <c r="B330">
-        <v>115.98716659483789</v>
+        <v>115.67878178422639</v>
       </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="1">
-        <v>34333.187540932333</v>
+        <v>34272.346939972434</v>
       </c>
       <c r="B331">
-        <v>118.09797442896135</v>
+        <v>115.67878178422639</v>
       </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332" s="1">
-        <v>34363.571322444113</v>
+        <v>34302.730721484222</v>
       </c>
       <c r="B332">
-        <v>116.6039362160609</v>
+        <v>115.98716659483789</v>
       </c>
     </row>
     <row r="333" spans="1:2">
       <c r="A333" s="1">
-        <v>34394.028141892224</v>
+        <v>34333.187540932333</v>
       </c>
       <c r="B333">
-        <v>115.67878178422639</v>
+        <v>118.09797442896135</v>
       </c>
     </row>
     <row r="334" spans="1:2">
       <c r="A334" s="1">
-        <v>34424.411923404012</v>
+        <v>34363.571322444113</v>
       </c>
       <c r="B334">
-        <v>115.72858305798975</v>
+        <v>116.6039362160609</v>
       </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="1">
-        <v>34454.868742852115</v>
+        <v>34394.028141892224</v>
       </c>
       <c r="B335">
-        <v>115.83393190633528</v>
+        <v>115.67878178422639</v>
       </c>
     </row>
     <row r="336" spans="1:2">
       <c r="A336" s="1">
-        <v>34485.252524363903</v>
+        <v>34424.411923404012</v>
       </c>
       <c r="B336">
-        <v>116.03888330220752</v>
+        <v>115.72858305798975</v>
       </c>
     </row>
     <row r="337" spans="1:2">
       <c r="A337" s="1">
-        <v>34515.709343812014</v>
+        <v>34454.868742852115</v>
       </c>
       <c r="B337">
-        <v>116.70736963080017</v>
+        <v>115.83393190633528</v>
       </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="1">
-        <v>34546.093125323794</v>
+        <v>34485.252524363903</v>
       </c>
       <c r="B338">
-        <v>117.78958961834985</v>
+        <v>116.03888330220752</v>
       </c>
     </row>
     <row r="339" spans="1:2">
       <c r="A339" s="1">
-        <v>34576.549944771905</v>
+        <v>34515.709343812014</v>
       </c>
       <c r="B339">
-        <v>117.01575444141167</v>
+        <v>116.70736963080017</v>
       </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340" s="1">
-        <v>34607.006764220016</v>
+        <v>34546.093125323794</v>
       </c>
       <c r="B340">
-        <v>117.58272278887132</v>
+        <v>117.78958961834985</v>
       </c>
     </row>
     <row r="341" spans="1:2">
       <c r="A341" s="1">
-        <v>34637.390545731796</v>
+        <v>34576.549944771905</v>
       </c>
       <c r="B341">
-        <v>119.9003974524733</v>
+        <v>117.01575444141167</v>
       </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342" s="1">
-        <v>34667.847365179907</v>
+        <v>34607.006764220016</v>
       </c>
       <c r="B342">
-        <v>119.9003974524733</v>
+        <v>117.58272278887132</v>
       </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343" s="1">
-        <v>34698.304184628018</v>
+        <v>34637.390545731796</v>
       </c>
       <c r="B343">
-        <v>121.7526217497486</v>
+        <v>119.9003974524733</v>
       </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344" s="1">
-        <v>34728.687966139798</v>
+        <v>34667.847365179907</v>
       </c>
       <c r="B344">
-        <v>123.29646123641238</v>
+        <v>119.9003974524733</v>
       </c>
     </row>
     <row r="345" spans="1:2">
       <c r="A345" s="1">
-        <v>34759.217823524239</v>
+        <v>34698.304184628018</v>
       </c>
       <c r="B345">
-        <v>121.28908681702821</v>
+        <v>121.7526217497486</v>
       </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346" s="1">
-        <v>34789.528567099696</v>
+        <v>34728.687966139798</v>
       </c>
       <c r="B346">
-        <v>124.63534932720394</v>
+        <v>123.29646123641238</v>
       </c>
     </row>
     <row r="347" spans="1:2">
       <c r="A347" s="1">
-        <v>34820.05842448413</v>
+        <v>34759.217823524239</v>
       </c>
       <c r="B347">
-        <v>123.70827946176315</v>
+        <v>121.28908681702821</v>
       </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348" s="1">
-        <v>34850.369168059588</v>
+        <v>34789.528567099696</v>
       </c>
       <c r="B348">
-        <v>123.55504477326055</v>
+        <v>124.63534932720394</v>
       </c>
     </row>
     <row r="349" spans="1:2">
       <c r="A349" s="1">
-        <v>34880.899025444029</v>
+        <v>34820.05842448413</v>
       </c>
       <c r="B349">
-        <v>124.37868122396208</v>
+        <v>123.70827946176315</v>
       </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350" s="1">
-        <v>34911.209769019479</v>
+        <v>34850.369168059588</v>
       </c>
       <c r="B350">
-        <v>124.7387827419432</v>
+        <v>123.55504477326055</v>
       </c>
     </row>
     <row r="351" spans="1:2">
       <c r="A351" s="1">
-        <v>34941.73962640392</v>
+        <v>34880.899025444029</v>
       </c>
       <c r="B351">
-        <v>120.72211846956856</v>
+        <v>124.37868122396208</v>
       </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352" s="1">
-        <v>34972.050369979377</v>
+        <v>34911.209769019479</v>
       </c>
       <c r="B352">
-        <v>124.48211463870132</v>
+        <v>124.7387827419432</v>
       </c>
     </row>
     <row r="353" spans="1:2">
       <c r="A353" s="1">
-        <v>35002.580227363811</v>
+        <v>34941.73962640392</v>
       </c>
       <c r="B353">
-        <v>122.88464301106163</v>
+        <v>120.72211846956856</v>
       </c>
     </row>
     <row r="354" spans="1:2">
       <c r="A354" s="1">
-        <v>35032.890970939268</v>
+        <v>34972.050369979377</v>
       </c>
       <c r="B354">
-        <v>122.98807642580088</v>
+        <v>124.48211463870132</v>
       </c>
     </row>
     <row r="355" spans="1:2">
       <c r="A355" s="1">
-        <v>35063.420828323709</v>
+        <v>35002.580227363811</v>
       </c>
       <c r="B355">
-        <v>123.19494325527941</v>
+        <v>122.88464301106163</v>
       </c>
     </row>
     <row r="356" spans="1:2">
       <c r="A356" s="1">
-        <v>35093.731571899159</v>
+        <v>35032.890970939268</v>
       </c>
       <c r="B356">
-        <v>123.91514629124167</v>
+        <v>122.98807642580088</v>
       </c>
     </row>
     <row r="357" spans="1:2">
       <c r="A357" s="1">
-        <v>35124.261429283601</v>
+        <v>35063.420828323709</v>
       </c>
       <c r="B357">
-        <v>128.96039841019009</v>
+        <v>123.19494325527941</v>
       </c>
     </row>
     <row r="358" spans="1:2">
       <c r="A358" s="1">
-        <v>35154.572172859058</v>
+        <v>35093.731571899159</v>
       </c>
       <c r="B358">
-        <v>123.75999616913279</v>
+        <v>123.91514629124167</v>
       </c>
     </row>
     <row r="359" spans="1:2">
       <c r="A359" s="1">
-        <v>35185.102030243492</v>
+        <v>35124.261429283601</v>
       </c>
       <c r="B359">
-        <v>121.23737010965857</v>
+        <v>128.96039841019009</v>
       </c>
     </row>
     <row r="360" spans="1:2">
       <c r="A360" s="1">
-        <v>35215.412773818949</v>
+        <v>35154.572172859058</v>
       </c>
       <c r="B360">
-        <v>120.92898529904707</v>
+        <v>123.75999616913279</v>
       </c>
     </row>
     <row r="361" spans="1:2">
       <c r="A361" s="1">
-        <v>35245.979150171552</v>
+        <v>35185.102030243492</v>
       </c>
       <c r="B361">
-        <v>122.11272326772973</v>
+        <v>121.23737010965857</v>
       </c>
     </row>
     <row r="362" spans="1:2">
       <c r="A362" s="1">
-        <v>35276.25337477884</v>
+        <v>35215.412773818949</v>
       </c>
       <c r="B362">
-        <v>121.64918833500933</v>
+        <v>120.92898529904707</v>
       </c>
     </row>
     <row r="363" spans="1:2">
       <c r="A363" s="1">
-        <v>35306.783232163281</v>
+        <v>35245.979150171552</v>
       </c>
       <c r="B363">
-        <v>123.19494325527941</v>
+        <v>122.11272326772973</v>
       </c>
     </row>
     <row r="364" spans="1:2">
       <c r="A364" s="1">
-        <v>35337.1304947069</v>
+        <v>35276.25337477884</v>
       </c>
       <c r="B364">
-        <v>124.22353110185317</v>
+        <v>121.64918833500933</v>
       </c>
     </row>
     <row r="365" spans="1:2">
       <c r="A365" s="1">
-        <v>35367.623833123173</v>
+        <v>35306.783232163281</v>
       </c>
       <c r="B365">
-        <v>120.67231719580519</v>
+        <v>123.19494325527941</v>
       </c>
     </row>
     <row r="366" spans="1:2">
       <c r="A366" s="1">
-        <v>35397.971095666799</v>
+        <v>35337.1304947069</v>
       </c>
       <c r="B366">
-        <v>117.94282430685246</v>
+        <v>124.22353110185317</v>
       </c>
     </row>
     <row r="367" spans="1:2">
       <c r="A367" s="1">
-        <v>35428.464434083071</v>
+        <v>35367.623833123173</v>
       </c>
       <c r="B367">
-        <v>117.89110759948284</v>
+        <v>120.67231719580519</v>
       </c>
     </row>
     <row r="368" spans="1:2">
       <c r="A368" s="1">
-        <v>35458.81169662669</v>
+        <v>35397.971095666799</v>
       </c>
       <c r="B368">
-        <v>116.45070152755829</v>
+        <v>117.94282430685246</v>
       </c>
     </row>
     <row r="369" spans="1:2">
       <c r="A369" s="1">
-        <v>35489.341554011124</v>
+        <v>35428.464434083071</v>
       </c>
       <c r="B369">
-        <v>117.63443949624096</v>
+        <v>117.89110759948284</v>
       </c>
     </row>
     <row r="370" spans="1:2">
       <c r="A370" s="1">
-        <v>35519.688816554743</v>
+        <v>35458.81169662669</v>
       </c>
       <c r="B370">
-        <v>115.98716659483789</v>
+        <v>116.45070152755829</v>
       </c>
     </row>
     <row r="371" spans="1:2">
       <c r="A371" s="1">
-        <v>35550.182154971015</v>
+        <v>35489.341554011124</v>
       </c>
       <c r="B371">
-        <v>118.50979265431212</v>
+        <v>117.63443949624096</v>
       </c>
     </row>
     <row r="372" spans="1:2">
       <c r="A372" s="1">
-        <v>35580.529417514641</v>
+        <v>35519.688816554743</v>
       </c>
       <c r="B372">
-        <v>119.59009720825551</v>
+        <v>115.98716659483789</v>
       </c>
     </row>
     <row r="373" spans="1:2">
       <c r="A373" s="1">
-        <v>35611.022755930913</v>
+        <v>35550.182154971015</v>
       </c>
       <c r="B373">
-        <v>118.61131063544509</v>
+        <v>118.50979265431212</v>
       </c>
     </row>
     <row r="374" spans="1:2">
       <c r="A374" s="1">
-        <v>35641.370018474532</v>
+        <v>35580.529417514641</v>
       </c>
       <c r="B374">
-        <v>117.5310060815017</v>
+        <v>119.59009720825551</v>
       </c>
     </row>
     <row r="375" spans="1:2">
       <c r="A375" s="1">
-        <v>35671.863356890804</v>
+        <v>35611.022755930913</v>
       </c>
       <c r="B375">
-        <v>118.25120911746396</v>
+        <v>118.61131063544509</v>
       </c>
     </row>
     <row r="376" spans="1:2">
       <c r="A376" s="1">
-        <v>35702.210619434423</v>
+        <v>35641.370018474532</v>
       </c>
       <c r="B376">
-        <v>116.75908633816979</v>
+        <v>117.5310060815017</v>
       </c>
     </row>
     <row r="377" spans="1:2">
       <c r="A377" s="1">
-        <v>35732.740476818864</v>
+        <v>35671.863356890804</v>
       </c>
       <c r="B377">
-        <v>119.84868074510366</v>
+        <v>118.25120911746396</v>
       </c>
     </row>
     <row r="378" spans="1:2">
       <c r="A378" s="1">
-        <v>35763.087739362483</v>
+        <v>35702.210619434423</v>
       </c>
       <c r="B378">
-        <v>119.33342910501365</v>
+        <v>116.75908633816979</v>
       </c>
     </row>
     <row r="379" spans="1:2">
       <c r="A379" s="1">
-        <v>35793.581077778756</v>
+        <v>35732.740476818864</v>
       </c>
       <c r="B379">
-        <v>118.76646075755399</v>
+        <v>119.84868074510366</v>
       </c>
     </row>
     <row r="380" spans="1:2">
       <c r="A380" s="1">
-        <v>35823.928340322374</v>
+        <v>35763.087739362483</v>
       </c>
       <c r="B380">
-        <v>118.76646075755399</v>
+        <v>119.33342910501365</v>
       </c>
     </row>
     <row r="381" spans="1:2">
       <c r="A381" s="1">
-        <v>35854.421678738654</v>
+        <v>35793.581077778756</v>
       </c>
       <c r="B381">
-        <v>117.68615620361059</v>
+        <v>118.76646075755399</v>
       </c>
     </row>
     <row r="382" spans="1:2">
       <c r="A382" s="1">
-        <v>35884.768941282273</v>
+        <v>35823.928340322374</v>
       </c>
       <c r="B382">
-        <v>118.09797442896135</v>
+        <v>118.76646075755399</v>
       </c>
     </row>
     <row r="383" spans="1:2">
       <c r="A383" s="1">
-        <v>35915.262279698545</v>
+        <v>35854.421678738654</v>
       </c>
       <c r="B383">
-        <v>118.71474405018436</v>
+        <v>117.68615620361059</v>
       </c>
     </row>
     <row r="384" spans="1:2">
       <c r="A384" s="1">
-        <v>35945.646061210326</v>
+        <v>35884.768941282273</v>
       </c>
       <c r="B384">
-        <v>118.61131063544509</v>
+        <v>118.09797442896135</v>
       </c>
     </row>
     <row r="385" spans="1:2">
       <c r="A385" s="1">
-        <v>35976.139399626598</v>
+        <v>35915.262279698545</v>
       </c>
       <c r="B385">
-        <v>115.06009672939712</v>
+        <v>118.71474405018436</v>
       </c>
     </row>
     <row r="386" spans="1:2">
       <c r="A386" s="1">
-        <v>36006.486662170224</v>
+        <v>35945.646061210326</v>
       </c>
       <c r="B386">
-        <v>115.31676483263898</v>
+        <v>118.61131063544509</v>
       </c>
     </row>
     <row r="387" spans="1:2">
       <c r="A387" s="1">
-        <v>36036.980000586496</v>
+        <v>35976.139399626598</v>
       </c>
       <c r="B387">
-        <v>114.90494660728821</v>
+        <v>115.06009672939712</v>
       </c>
     </row>
     <row r="388" spans="1:2">
       <c r="A388" s="1">
-        <v>36068.349794238682</v>
+        <v>36006.486662170224</v>
       </c>
       <c r="B388">
-        <v>115.21524685150601</v>
+        <v>115.31676483263898</v>
       </c>
     </row>
     <row r="389" spans="1:2">
       <c r="A389" s="1">
-        <v>36098.73357575047</v>
+        <v>36036.980000586496</v>
       </c>
       <c r="B389">
-        <v>115.00838002202748</v>
+        <v>114.90494660728821</v>
       </c>
     </row>
     <row r="390" spans="1:2">
       <c r="A390" s="1">
-        <v>36129.263433134904</v>
+        <v>36068.349794238682</v>
       </c>
       <c r="B390">
-        <v>115.67878178422639</v>
+        <v>115.21524685150601</v>
       </c>
     </row>
     <row r="391" spans="1:2">
       <c r="A391" s="1">
-        <v>36159.647214646684</v>
+        <v>36098.73357575047</v>
       </c>
       <c r="B391">
-        <v>115.52363166211752</v>
+        <v>115.00838002202748</v>
       </c>
     </row>
     <row r="392" spans="1:2">
       <c r="A392" s="1">
-        <v>36190.104034094795</v>
+        <v>36129.263433134904</v>
       </c>
       <c r="B392">
-        <v>115.42019824737825</v>
+        <v>115.67878178422639</v>
       </c>
     </row>
     <row r="393" spans="1:2">
       <c r="A393" s="1">
-        <v>36220.487815606582</v>
+        <v>36159.647214646684</v>
       </c>
       <c r="B393">
-        <v>115.78029976535939</v>
+        <v>115.52363166211752</v>
       </c>
     </row>
     <row r="394" spans="1:2">
       <c r="A394" s="1">
-        <v>36250.944635054693</v>
+        <v>36190.104034094795</v>
       </c>
       <c r="B394">
-        <v>115.88373318009863</v>
+        <v>115.42019824737825</v>
       </c>
     </row>
     <row r="395" spans="1:2">
       <c r="A395" s="1">
-        <v>36281.328416566474</v>
+        <v>36220.487815606582</v>
       </c>
       <c r="B395">
-        <v>113.36110712062442</v>
+        <v>115.78029976535939</v>
       </c>
     </row>
     <row r="396" spans="1:2">
       <c r="A396" s="1">
-        <v>36311.785236014584</v>
+        <v>36250.944635054693</v>
       </c>
       <c r="B396">
-        <v>112.53747066992288</v>
+        <v>115.88373318009863</v>
       </c>
     </row>
     <row r="397" spans="1:2">
       <c r="A397" s="1">
-        <v>36342.169017526372</v>
+        <v>36281.328416566474</v>
       </c>
       <c r="B397">
-        <v>112.48766939615955</v>
+        <v>113.36110712062442</v>
       </c>
     </row>
     <row r="398" spans="1:2">
       <c r="A398" s="1">
-        <v>36372.625836974476</v>
+        <v>36311.785236014584</v>
       </c>
       <c r="B398">
-        <v>112.74433749940141</v>
+        <v>112.53747066992288</v>
       </c>
     </row>
     <row r="399" spans="1:2">
       <c r="A399" s="1">
-        <v>36403.009618486263</v>
+        <v>36342.169017526372</v>
       </c>
       <c r="B399">
-        <v>113.15615572475218</v>
+        <v>112.48766939615955</v>
       </c>
     </row>
     <row r="400" spans="1:2">
       <c r="A400" s="1">
-        <v>36433.466437934374</v>
+        <v>36372.625836974476</v>
       </c>
       <c r="B400">
-        <v>112.79413877316476</v>
+        <v>112.74433749940141</v>
       </c>
     </row>
     <row r="401" spans="1:2">
       <c r="A401" s="1">
-        <v>36463.850219446154</v>
+        <v>36403.009618486263</v>
       </c>
       <c r="B401">
-        <v>111.25029928650096</v>
+        <v>113.15615572475218</v>
       </c>
     </row>
     <row r="402" spans="1:2">
       <c r="A402" s="1">
-        <v>36494.307038894265</v>
+        <v>36433.466437934374</v>
       </c>
       <c r="B402">
-        <v>108.52272183115454</v>
+        <v>112.79413877316476</v>
       </c>
     </row>
     <row r="403" spans="1:2">
       <c r="A403" s="1">
-        <v>36555.220677790487</v>
+        <v>36463.850219446154</v>
       </c>
       <c r="B403">
-        <v>108.0074701910645</v>
+        <v>111.25029928650096</v>
       </c>
     </row>
     <row r="404" spans="1:2">
       <c r="A404" s="1">
-        <v>36585.531421365944</v>
+        <v>36494.307038894265</v>
       </c>
       <c r="B404">
-        <v>107.699085380453</v>
+        <v>108.52272183115454</v>
       </c>
     </row>
     <row r="405" spans="1:2">
       <c r="A405" s="1">
-        <v>36616.061278750378</v>
+        <v>36555.220677790487</v>
       </c>
       <c r="B405">
-        <v>107.44241727721112</v>
+        <v>108.0074701910645</v>
       </c>
     </row>
     <row r="406" spans="1:2">
       <c r="A406" s="1">
-        <v>36646.408541294004</v>
+        <v>36585.531421365944</v>
       </c>
       <c r="B406">
-        <v>107.08040032562371</v>
+        <v>107.699085380453</v>
       </c>
     </row>
     <row r="407" spans="1:2">
       <c r="A407" s="1">
-        <v>36676.901879710276</v>
+        <v>36616.061278750378</v>
       </c>
       <c r="B407">
-        <v>106.82373222238184</v>
+        <v>107.44241727721112</v>
       </c>
     </row>
     <row r="408" spans="1:2">
       <c r="A408" s="1">
-        <v>36707.249142253895</v>
+        <v>36646.408541294004</v>
       </c>
       <c r="B408">
-        <v>107.18383374036299</v>
+        <v>107.08040032562371</v>
       </c>
     </row>
     <row r="409" spans="1:2">
       <c r="A409" s="1">
-        <v>36737.742480670167</v>
+        <v>36676.901879710276</v>
       </c>
       <c r="B409">
-        <v>107.49413398458074</v>
+        <v>106.82373222238184</v>
       </c>
     </row>
     <row r="410" spans="1:2">
       <c r="A410" s="1">
-        <v>36768.089743213786</v>
+        <v>36707.249142253895</v>
       </c>
       <c r="B410">
-        <v>107.44241727721112</v>
+        <v>107.18383374036299</v>
       </c>
     </row>
     <row r="411" spans="1:2">
       <c r="A411" s="1">
-        <v>36798.583081630059</v>
+        <v>36737.742480670167</v>
       </c>
       <c r="B411">
-        <v>107.28726715510223</v>
+        <v>107.49413398458074</v>
       </c>
     </row>
     <row r="412" spans="1:2">
       <c r="A412" s="1">
-        <v>36828.930344173685</v>
+        <v>36768.089743213786</v>
       </c>
       <c r="B412">
         <v>107.44241727721112</v>
@@ -45708,535 +45716,535 @@
     </row>
     <row r="413" spans="1:2">
       <c r="A413" s="1">
-        <v>36859.423682589957</v>
+        <v>36798.583081630059</v>
       </c>
       <c r="B413">
-        <v>107.90403677632523</v>
+        <v>107.28726715510223</v>
       </c>
     </row>
     <row r="414" spans="1:2">
       <c r="A414" s="1">
-        <v>36889.807464101737</v>
+        <v>36828.930344173685</v>
       </c>
       <c r="B414">
-        <v>107.85423550256189</v>
+        <v>107.44241727721112</v>
       </c>
     </row>
     <row r="415" spans="1:2">
       <c r="A415" s="1">
-        <v>36920.264283549848</v>
+        <v>36859.423682589957</v>
       </c>
       <c r="B415">
-        <v>108.41928841641527</v>
+        <v>107.90403677632523</v>
       </c>
     </row>
     <row r="416" spans="1:2">
       <c r="A416" s="1">
-        <v>36950.648065061629</v>
+        <v>36889.807464101737</v>
       </c>
       <c r="B416">
-        <v>108.88282334913566</v>
+        <v>107.85423550256189</v>
       </c>
     </row>
     <row r="417" spans="1:2">
       <c r="A417" s="1">
-        <v>36981.104884509739</v>
+        <v>36920.264283549848</v>
       </c>
       <c r="B417">
-        <v>108.26413829430638</v>
+        <v>108.41928841641527</v>
       </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" s="1">
-        <v>37011.671260862342</v>
+        <v>36950.648065061629</v>
       </c>
       <c r="B418">
-        <v>107.95575348369485</v>
+        <v>108.88282334913566</v>
       </c>
     </row>
     <row r="419" spans="1:2">
       <c r="A419" s="1">
-        <v>37041.982004437799</v>
+        <v>36981.104884509739</v>
       </c>
       <c r="B419">
-        <v>107.90403677632523</v>
+        <v>108.26413829430638</v>
       </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" s="1">
-        <v>37072.329266981418</v>
+        <v>37011.671260862342</v>
       </c>
       <c r="B420">
-        <v>107.90403677632523</v>
+        <v>107.95575348369485</v>
       </c>
     </row>
     <row r="421" spans="1:2">
       <c r="A421" s="1">
-        <v>37102.82260539769</v>
+        <v>37041.982004437799</v>
       </c>
       <c r="B421">
-        <v>107.75080208782262</v>
+        <v>107.90403677632523</v>
       </c>
     </row>
     <row r="422" spans="1:2">
       <c r="A422" s="1">
-        <v>37133.31594381397</v>
+        <v>37072.329266981418</v>
       </c>
       <c r="B422">
-        <v>107.13403246659962</v>
+        <v>107.90403677632523</v>
       </c>
     </row>
     <row r="423" spans="1:2">
       <c r="A423" s="1">
-        <v>37163.663206357589</v>
+        <v>37102.82260539769</v>
       </c>
       <c r="B423">
-        <v>106.41191399703106</v>
+        <v>107.75080208782262</v>
       </c>
     </row>
     <row r="424" spans="1:2">
       <c r="A424" s="1">
-        <v>37194.193063742023</v>
+        <v>37133.31594381397</v>
       </c>
       <c r="B424">
-        <v>106.05181247904994</v>
+        <v>107.13403246659962</v>
       </c>
     </row>
     <row r="425" spans="1:2">
       <c r="A425" s="1">
-        <v>37224.50380731748</v>
+        <v>37163.663206357589</v>
       </c>
       <c r="B425">
-        <v>106.10352918641956</v>
+        <v>106.41191399703106</v>
       </c>
     </row>
     <row r="426" spans="1:2">
       <c r="A426" s="1">
-        <v>37255.033664701914</v>
+        <v>37194.193063742023</v>
       </c>
       <c r="B426">
-        <v>105.38141071685104</v>
+        <v>106.05181247904994</v>
       </c>
     </row>
     <row r="427" spans="1:2">
       <c r="A427" s="1">
-        <v>37285.38092724554</v>
+        <v>37224.50380731748</v>
       </c>
       <c r="B427">
-        <v>105.27797730211176</v>
+        <v>106.10352918641956</v>
       </c>
     </row>
     <row r="428" spans="1:2">
       <c r="A428" s="1">
-        <v>37315.874265661812</v>
+        <v>37255.033664701914</v>
       </c>
       <c r="B428">
-        <v>104.6114064071254</v>
+        <v>105.38141071685104</v>
       </c>
     </row>
     <row r="429" spans="1:2">
       <c r="A429" s="1">
-        <v>37346.221528205431</v>
+        <v>37285.38092724554</v>
       </c>
       <c r="B429">
-        <v>104.66120768088877</v>
+        <v>105.27797730211176</v>
       </c>
     </row>
     <row r="430" spans="1:2">
       <c r="A430" s="1">
-        <v>37376.714866621704</v>
+        <v>37315.874265661812</v>
       </c>
       <c r="B430">
-        <v>104.76464109562801</v>
+        <v>104.6114064071254</v>
       </c>
     </row>
     <row r="431" spans="1:2">
       <c r="A431" s="1">
-        <v>37407.062129165322</v>
+        <v>37346.221528205431</v>
       </c>
       <c r="B431">
-        <v>104.76464109562801</v>
+        <v>104.66120768088877</v>
       </c>
     </row>
     <row r="432" spans="1:2">
       <c r="A432" s="1">
-        <v>37437.591986549756</v>
+        <v>37376.714866621704</v>
       </c>
       <c r="B432">
-        <v>104.86807451036728</v>
+        <v>104.76464109562801</v>
       </c>
     </row>
     <row r="433" spans="1:2">
       <c r="A433" s="1">
-        <v>37467.902730125221</v>
+        <v>37407.062129165322</v>
       </c>
       <c r="B433">
-        <v>104.81635780299766</v>
+        <v>104.76464109562801</v>
       </c>
     </row>
     <row r="434" spans="1:2">
       <c r="A434" s="1">
-        <v>37498.432587509655</v>
+        <v>37437.591986549756</v>
       </c>
       <c r="B434">
-        <v>105.12474261360916</v>
+        <v>104.86807451036728</v>
       </c>
     </row>
     <row r="435" spans="1:2">
       <c r="A435" s="1">
-        <v>37528.779850053274</v>
+        <v>37467.902730125221</v>
       </c>
       <c r="B435">
-        <v>104.86807451036728</v>
+        <v>104.81635780299766</v>
       </c>
     </row>
     <row r="436" spans="1:2">
       <c r="A436" s="1">
-        <v>37559.273188469546</v>
+        <v>37498.432587509655</v>
       </c>
       <c r="B436">
-        <v>105.02322463247617</v>
+        <v>105.12474261360916</v>
       </c>
     </row>
     <row r="437" spans="1:2">
       <c r="A437" s="1">
-        <v>37589.620451013165</v>
+        <v>37528.779850053274</v>
       </c>
       <c r="B437">
-        <v>104.66120768088877</v>
+        <v>104.86807451036728</v>
       </c>
     </row>
     <row r="438" spans="1:2">
       <c r="A438" s="1">
-        <v>37620.113789429437</v>
+        <v>37559.273188469546</v>
       </c>
       <c r="B438">
-        <v>105.17645932097878</v>
+        <v>105.02322463247617</v>
       </c>
     </row>
     <row r="439" spans="1:2">
       <c r="A439" s="1">
-        <v>37650.461051973063</v>
+        <v>37589.620451013165</v>
       </c>
       <c r="B439">
-        <v>104.6114064071254</v>
+        <v>104.66120768088877</v>
       </c>
     </row>
     <row r="440" spans="1:2">
       <c r="A440" s="1">
-        <v>37680.990909357497</v>
+        <v>37620.113789429437</v>
       </c>
       <c r="B440">
-        <v>104.66120768088877</v>
+        <v>105.17645932097878</v>
       </c>
     </row>
     <row r="441" spans="1:2">
       <c r="A441" s="1">
-        <v>37711.338171901116</v>
+        <v>37650.461051973063</v>
       </c>
       <c r="B441">
-        <v>104.96959249150026</v>
+        <v>104.6114064071254</v>
       </c>
     </row>
     <row r="442" spans="1:2">
       <c r="A442" s="1">
-        <v>37741.831510317395</v>
+        <v>37680.990909357497</v>
       </c>
       <c r="B442">
-        <v>104.50797299238616</v>
+        <v>104.66120768088877</v>
       </c>
     </row>
     <row r="443" spans="1:2">
       <c r="A443" s="1">
-        <v>37772.178772861007</v>
+        <v>37711.338171901116</v>
       </c>
       <c r="B443">
-        <v>105.43312742422066</v>
+        <v>104.96959249150026</v>
       </c>
     </row>
     <row r="444" spans="1:2">
       <c r="A444" s="1">
-        <v>37802.672111277287</v>
+        <v>37741.831510317395</v>
       </c>
       <c r="B444">
-        <v>104.71292438825839</v>
+        <v>104.50797299238616</v>
       </c>
     </row>
     <row r="445" spans="1:2">
       <c r="A445" s="1">
-        <v>37833.019373820905</v>
+        <v>37772.178772861007</v>
       </c>
       <c r="B445">
-        <v>103.58090312694537</v>
+        <v>105.43312742422066</v>
       </c>
     </row>
     <row r="446" spans="1:2">
       <c r="A446" s="1">
-        <v>37863.549231205339</v>
+        <v>37802.672111277287</v>
       </c>
       <c r="B446">
-        <v>103.73413781544798</v>
+        <v>104.71292438825839</v>
       </c>
     </row>
     <row r="447" spans="1:2">
       <c r="A447" s="1">
-        <v>37893.859974780797</v>
+        <v>37833.019373820905</v>
       </c>
       <c r="B447">
-        <v>104.40453957764689</v>
+        <v>103.58090312694537</v>
       </c>
     </row>
     <row r="448" spans="1:2">
       <c r="A448" s="1">
-        <v>37924.389832165238</v>
+        <v>37863.549231205339</v>
       </c>
       <c r="B448">
-        <v>104.19767274816834</v>
+        <v>103.73413781544798</v>
       </c>
     </row>
     <row r="449" spans="1:2">
       <c r="A449" s="1">
-        <v>37954.773613677018</v>
+        <v>37893.859974780797</v>
       </c>
       <c r="B449">
-        <v>104.50797299238616</v>
+        <v>104.40453957764689</v>
       </c>
     </row>
     <row r="450" spans="1:2">
       <c r="A450" s="1">
-        <v>37985.230433125129</v>
+        <v>37924.389832165238</v>
       </c>
       <c r="B450">
-        <v>103.42575300483648</v>
+        <v>104.19767274816834</v>
       </c>
     </row>
     <row r="451" spans="1:2">
       <c r="A451" s="1">
-        <v>38046.07103408502</v>
+        <v>37954.773613677018</v>
       </c>
       <c r="B451">
-        <v>103.01393477948571</v>
+        <v>104.50797299238616</v>
       </c>
     </row>
     <row r="452" spans="1:2">
       <c r="A452" s="1">
-        <v>38076.454815596808</v>
+        <v>37985.230433125129</v>
       </c>
       <c r="B452">
-        <v>102.70554996887421</v>
+        <v>103.42575300483648</v>
       </c>
     </row>
     <row r="453" spans="1:2">
       <c r="A453" s="1">
-        <v>38106.94815401308</v>
+        <v>38046.07103408502</v>
       </c>
       <c r="B453">
-        <v>103.27060288272759</v>
+        <v>103.01393477948571</v>
       </c>
     </row>
     <row r="454" spans="1:2">
       <c r="A454" s="1">
-        <v>38137.295416556699</v>
+        <v>38076.454815596808</v>
       </c>
       <c r="B454">
-        <v>103.27060288272759</v>
+        <v>102.70554996887421</v>
       </c>
     </row>
     <row r="455" spans="1:2">
       <c r="A455" s="1">
-        <v>38167.82527394114</v>
+        <v>38106.94815401308</v>
       </c>
       <c r="B455">
-        <v>102.80706795000717</v>
+        <v>103.27060288272759</v>
       </c>
     </row>
     <row r="456" spans="1:2">
       <c r="A456" s="1">
-        <v>38198.172536484759</v>
+        <v>38137.295416556699</v>
       </c>
       <c r="B456">
-        <v>102.24201503615379</v>
+        <v>103.27060288272759</v>
       </c>
     </row>
     <row r="457" spans="1:2">
       <c r="A457" s="1">
-        <v>38228.665874901031</v>
+        <v>38167.82527394114</v>
       </c>
       <c r="B457">
-        <v>102.29373174352344</v>
+        <v>102.80706795000717</v>
       </c>
     </row>
     <row r="458" spans="1:2">
       <c r="A458" s="1">
-        <v>38259.01313744465</v>
+        <v>38198.172536484759</v>
       </c>
       <c r="B458">
-        <v>102.19029832878419</v>
+        <v>102.24201503615379</v>
       </c>
     </row>
     <row r="459" spans="1:2">
       <c r="A459" s="1">
-        <v>38289.506475860922</v>
+        <v>38228.665874901031</v>
       </c>
       <c r="B459">
-        <v>102.08878034765118</v>
+        <v>102.29373174352344</v>
       </c>
     </row>
     <row r="460" spans="1:2">
       <c r="A460" s="1">
-        <v>38319.853738404548</v>
+        <v>38259.01313744465</v>
       </c>
       <c r="B460">
-        <v>102.96221807211606</v>
+        <v>102.19029832878419</v>
       </c>
     </row>
     <row r="461" spans="1:2">
       <c r="A461" s="1">
-        <v>38350.347076820821</v>
+        <v>38289.506475860922</v>
       </c>
       <c r="B461">
-        <v>102.24201503615379</v>
+        <v>102.08878034765118</v>
       </c>
     </row>
     <row r="462" spans="1:2">
       <c r="A462" s="1">
-        <v>38380.69433936444</v>
+        <v>38319.853738404548</v>
       </c>
       <c r="B462">
-        <v>108.05918689843412</v>
+        <v>102.96221807211606</v>
       </c>
     </row>
     <row r="463" spans="1:2">
       <c r="A463" s="1">
-        <v>38411.224196748874</v>
+        <v>38350.347076820821</v>
       </c>
       <c r="B463">
-        <v>107.18383374036299</v>
+        <v>102.24201503615379</v>
       </c>
     </row>
     <row r="464" spans="1:2">
       <c r="A464" s="1">
-        <v>38441.571459292492</v>
+        <v>38380.69433936444</v>
       </c>
       <c r="B464">
-        <v>108.11090360580377</v>
+        <v>108.05918689843412</v>
       </c>
     </row>
     <row r="465" spans="1:2">
       <c r="A465" s="1">
-        <v>38472.064797708765</v>
+        <v>38411.224196748874</v>
       </c>
       <c r="B465">
-        <v>102.13858162141454</v>
+        <v>107.18383374036299</v>
       </c>
     </row>
     <row r="466" spans="1:2">
       <c r="A466" s="1">
-        <v>38502.412060252391</v>
+        <v>38441.571459292492</v>
       </c>
       <c r="B466">
-        <v>103.11736819422498</v>
+        <v>108.11090360580377</v>
       </c>
     </row>
     <row r="467" spans="1:2">
       <c r="A467" s="1">
-        <v>38532.905398668663</v>
+        <v>38472.064797708765</v>
       </c>
       <c r="B467">
-        <v>108.67595651965715</v>
+        <v>102.13858162141454</v>
       </c>
     </row>
     <row r="468" spans="1:2">
       <c r="A468" s="1">
-        <v>38563.252661212282</v>
+        <v>38502.412060252391</v>
       </c>
       <c r="B468">
-        <v>107.85423550256189</v>
+        <v>103.11736819422498</v>
       </c>
     </row>
     <row r="469" spans="1:2">
       <c r="A469" s="1">
-        <v>38593.782518596723</v>
+        <v>38532.905398668663</v>
       </c>
       <c r="B469">
-        <v>105.53656083895993</v>
+        <v>108.67595651965715</v>
       </c>
     </row>
     <row r="470" spans="1:2">
       <c r="A470" s="1">
-        <v>38624.093262172173</v>
+        <v>38563.252661212282</v>
       </c>
       <c r="B470">
-        <v>106.36019728966144</v>
+        <v>107.85423550256189</v>
       </c>
     </row>
     <row r="471" spans="1:2">
       <c r="A471" s="1">
-        <v>38654.623119556614</v>
+        <v>38593.782518596723</v>
       </c>
       <c r="B471">
-        <v>106.51343197816405</v>
+        <v>105.53656083895993</v>
       </c>
     </row>
     <row r="472" spans="1:2">
       <c r="A472" s="1">
-        <v>38684.970382100233</v>
+        <v>38624.093262172173</v>
       </c>
       <c r="B472">
-        <v>107.03059905186035</v>
+        <v>106.36019728966144</v>
       </c>
     </row>
     <row r="473" spans="1:2">
       <c r="A473" s="1">
-        <v>38715.463720516505</v>
+        <v>38654.623119556614</v>
       </c>
       <c r="B473">
-        <v>107.23555044773261</v>
+        <v>106.51343197816405</v>
       </c>
     </row>
     <row r="474" spans="1:2">
       <c r="A474" s="1">
-        <v>38745.810983060124</v>
+        <v>38684.970382100233</v>
       </c>
       <c r="B474">
-        <v>106.20504716755255</v>
+        <v>107.03059905186035</v>
       </c>
     </row>
     <row r="475" spans="1:2">
       <c r="A475" s="1">
-        <v>38776.304321476404</v>
+        <v>38715.463720516505</v>
       </c>
       <c r="B475">
-        <v>105.8449456495714</v>
+        <v>107.23555044773261</v>
       </c>
     </row>
     <row r="476" spans="1:2">
       <c r="A476" s="1">
-        <v>38806.651584020015</v>
+        <v>38745.810983060124</v>
       </c>
       <c r="B476">
-        <v>105.22817602834843</v>
+        <v>106.20504716755255</v>
       </c>
     </row>
     <row r="477" spans="1:2">
       <c r="A477" s="1">
-        <v>38837.181441404457</v>
+        <v>38776.304321476404</v>
       </c>
       <c r="B477">
-        <v>104.96959249150026</v>
+        <v>105.8449456495714</v>
       </c>
     </row>
     <row r="478" spans="1:2">
       <c r="A478" s="1">
-        <v>38867.528703948075</v>
+        <v>38806.651584020015</v>
       </c>
       <c r="B478">
-        <v>105.17645932097878</v>
+        <v>105.22817602834843</v>
       </c>
     </row>
     <row r="479" spans="1:2">
       <c r="A479" s="1">
-        <v>38898.022042364348</v>
+        <v>38837.181441404457</v>
       </c>
       <c r="B479">
         <v>104.96959249150026</v>
@@ -46244,38 +46252,55 @@
     </row>
     <row r="480" spans="1:2">
       <c r="A480" s="1">
-        <v>38928.369304907974</v>
+        <v>38867.528703948075</v>
       </c>
       <c r="B480">
-        <v>104.71292438825839</v>
+        <v>105.17645932097878</v>
       </c>
     </row>
     <row r="481" spans="1:2">
       <c r="A481" s="1">
-        <v>38958.862643324246</v>
+        <v>38898.022042364348</v>
       </c>
       <c r="B481">
-        <v>105.02322463247617</v>
+        <v>104.96959249150026</v>
       </c>
     </row>
     <row r="482" spans="1:2">
       <c r="A482" s="1">
-        <v>38989.209905867865</v>
+        <v>38928.369304907974</v>
       </c>
       <c r="B482">
-        <v>104.96959249150026</v>
+        <v>104.71292438825839</v>
       </c>
     </row>
     <row r="483" spans="1:2">
       <c r="A483" s="1">
+        <v>38958.862643324246</v>
+      </c>
+      <c r="B483">
+        <v>105.02322463247617</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="A484" s="1">
+        <v>38989.209905867865</v>
+      </c>
+      <c r="B484">
+        <v>104.96959249150026</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2">
+      <c r="A485" s="1">
         <v>39019.703244284137</v>
       </c>
-      <c r="B483">
+      <c r="B485">
         <v>104.71292438825839</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>